<commit_message>
Big changes on dataset structure. 5-fold CV splitting on time series.
</commit_message>
<xml_diff>
--- a/Dataset/Captions collection/5-Fold_Cross_Validation/Evaluation_results/BL0_Evaluation_Results.xlsx
+++ b/Dataset/Captions collection/5-Fold_Cross_Validation/Evaluation_results/BL0_Evaluation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\UBC Research Period\Research\Data Chart Captioning System\Dataset\Captions collection\5-Fold_Cross_Validation\Evaluation_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D98AEF-BE12-47B1-BF5E-CA3E279197B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB34438-7AC8-4007-82D7-F14404C6538C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46050" yWindow="3630" windowWidth="4185" windowHeight="2490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>